<commit_message>
Fix column position for 2015
</commit_message>
<xml_diff>
--- a/Budget/sql_2014.xlsx
+++ b/Budget/sql_2014.xlsx
@@ -432,7 +432,7 @@
   <dimension ref="A1:N43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -442,284 +442,284 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>12</v>
-      </c>
-      <c r="N1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>14</v>
       </c>
-      <c r="B2">
+      <c r="B2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2">
         <v>1141</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>2117</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>2609</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>2642</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>2240</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>2462</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>2584</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>2733</v>
       </c>
-      <c r="J2">
+      <c r="K2">
         <v>3319</v>
       </c>
-      <c r="K2">
+      <c r="L2">
         <v>3262</v>
       </c>
-      <c r="L2">
+      <c r="M2">
         <v>3467</v>
       </c>
-      <c r="M2">
+      <c r="N2">
         <v>3936</v>
-      </c>
-      <c r="N2" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>15</v>
       </c>
-      <c r="B3">
+      <c r="B3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3">
         <v>43</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>31</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>27</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>17</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>21</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>41</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>34</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>9</v>
       </c>
-      <c r="J3">
+      <c r="K3">
         <v>21</v>
       </c>
-      <c r="K3">
+      <c r="L3">
         <v>23</v>
       </c>
-      <c r="L3">
+      <c r="M3">
         <v>22</v>
       </c>
-      <c r="M3">
+      <c r="N3">
         <v>26</v>
-      </c>
-      <c r="N3" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>16</v>
       </c>
-      <c r="B4">
-        <v>0</v>
+      <c r="B4" t="s">
+        <v>28</v>
       </c>
       <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
         <v>612</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>1092</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>744</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>415</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>821</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>398</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>440</v>
       </c>
-      <c r="J4">
+      <c r="K4">
         <v>2076</v>
       </c>
-      <c r="K4">
+      <c r="L4">
         <v>1654</v>
       </c>
-      <c r="L4">
+      <c r="M4">
         <v>1474</v>
       </c>
-      <c r="M4">
+      <c r="N4">
         <v>1381</v>
-      </c>
-      <c r="N4" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>17</v>
       </c>
-      <c r="B5">
+      <c r="B5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5">
         <v>36</v>
       </c>
-      <c r="C5">
+      <c r="D5">
         <v>188</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>281</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>203</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>358</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>691</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>377</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>310</v>
       </c>
-      <c r="J5">
+      <c r="K5">
         <v>1346</v>
       </c>
-      <c r="K5">
+      <c r="L5">
         <v>1217</v>
       </c>
-      <c r="L5">
+      <c r="M5">
         <v>2060</v>
       </c>
-      <c r="M5">
+      <c r="N5">
         <v>1733</v>
-      </c>
-      <c r="N5" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>18</v>
       </c>
-      <c r="B6">
+      <c r="B6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6">
         <v>157</v>
       </c>
-      <c r="C6">
+      <c r="D6">
         <v>163</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <v>160</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>137</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>247</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>395</v>
       </c>
-      <c r="H6">
+      <c r="I6">
         <v>285</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <v>202</v>
       </c>
-      <c r="J6">
+      <c r="K6">
         <v>715</v>
       </c>
-      <c r="K6">
+      <c r="L6">
         <v>633</v>
       </c>
-      <c r="L6">
+      <c r="M6">
         <v>933</v>
       </c>
-      <c r="M6">
+      <c r="N6">
         <v>657</v>
-      </c>
-      <c r="N6" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>19</v>
       </c>
-      <c r="B7">
-        <v>0</v>
+      <c r="B7" t="s">
+        <v>28</v>
       </c>
       <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
         <v>5</v>
       </c>
-      <c r="D7">
+      <c r="E7">
         <v>24</v>
       </c>
-      <c r="E7">
+      <c r="F7">
         <v>6</v>
       </c>
-      <c r="F7">
-        <v>0</v>
-      </c>
       <c r="G7">
         <v>0</v>
       </c>
@@ -730,71 +730,71 @@
         <v>0</v>
       </c>
       <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
         <v>9</v>
       </c>
-      <c r="K7">
-        <v>0</v>
-      </c>
       <c r="L7">
         <v>0</v>
       </c>
       <c r="M7">
         <v>0</v>
       </c>
-      <c r="N7" t="s">
-        <v>28</v>
+      <c r="N7">
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>20</v>
       </c>
-      <c r="B8">
-        <v>0</v>
+      <c r="B8" t="s">
+        <v>28</v>
       </c>
       <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
         <v>76</v>
       </c>
-      <c r="D8">
+      <c r="E8">
         <v>704</v>
       </c>
-      <c r="E8">
+      <c r="F8">
         <v>323</v>
       </c>
-      <c r="F8">
+      <c r="G8">
         <v>245</v>
       </c>
-      <c r="G8">
+      <c r="H8">
         <v>461</v>
       </c>
-      <c r="H8">
+      <c r="I8">
         <v>241</v>
       </c>
-      <c r="I8">
+      <c r="J8">
         <v>227</v>
       </c>
-      <c r="J8">
+      <c r="K8">
         <v>1210</v>
       </c>
-      <c r="K8">
+      <c r="L8">
         <v>927</v>
       </c>
-      <c r="L8">
+      <c r="M8">
         <v>827</v>
       </c>
-      <c r="M8">
+      <c r="N8">
         <v>757</v>
-      </c>
-      <c r="N8" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>21</v>
       </c>
-      <c r="B9">
-        <v>0</v>
+      <c r="B9" t="s">
+        <v>28</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -818,247 +818,247 @@
         <v>0</v>
       </c>
       <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
         <v>4</v>
       </c>
-      <c r="K9">
+      <c r="L9">
         <v>16</v>
       </c>
-      <c r="L9">
+      <c r="M9">
         <v>20</v>
       </c>
-      <c r="M9">
+      <c r="N9">
         <v>7</v>
-      </c>
-      <c r="N9" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>22</v>
       </c>
-      <c r="B10">
+      <c r="B10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10">
         <v>509</v>
       </c>
-      <c r="C10">
+      <c r="D10">
         <v>514</v>
       </c>
-      <c r="D10">
+      <c r="E10">
         <v>594</v>
       </c>
-      <c r="E10">
+      <c r="F10">
         <v>519</v>
       </c>
-      <c r="F10">
+      <c r="G10">
         <v>771</v>
       </c>
-      <c r="G10">
+      <c r="H10">
         <v>1023</v>
       </c>
-      <c r="H10">
+      <c r="I10">
         <v>715</v>
       </c>
-      <c r="I10">
+      <c r="J10">
         <v>649</v>
       </c>
-      <c r="J10">
+      <c r="K10">
         <v>1514</v>
       </c>
-      <c r="K10">
+      <c r="L10">
         <v>1267</v>
       </c>
-      <c r="L10">
+      <c r="M10">
         <v>1879</v>
       </c>
-      <c r="M10">
+      <c r="N10">
         <v>1667</v>
-      </c>
-      <c r="N10" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>23</v>
       </c>
-      <c r="B11">
+      <c r="B11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11">
         <v>16</v>
       </c>
-      <c r="C11">
+      <c r="D11">
         <v>23</v>
       </c>
-      <c r="D11">
+      <c r="E11">
         <v>103</v>
       </c>
-      <c r="E11">
+      <c r="F11">
         <v>50</v>
       </c>
-      <c r="F11">
+      <c r="G11">
         <v>13</v>
       </c>
-      <c r="G11">
+      <c r="H11">
         <v>94</v>
       </c>
-      <c r="H11">
+      <c r="I11">
         <v>45</v>
       </c>
-      <c r="I11">
+      <c r="J11">
         <v>16</v>
       </c>
-      <c r="J11">
+      <c r="K11">
         <v>123</v>
       </c>
-      <c r="K11">
+      <c r="L11">
         <v>52</v>
       </c>
-      <c r="L11">
+      <c r="M11">
         <v>16</v>
       </c>
-      <c r="M11">
+      <c r="N11">
         <v>6</v>
-      </c>
-      <c r="N11" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>24</v>
       </c>
-      <c r="B12">
+      <c r="B12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12">
         <v>163</v>
       </c>
-      <c r="C12">
+      <c r="D12">
         <v>142</v>
       </c>
-      <c r="D12">
+      <c r="E12">
         <v>150</v>
       </c>
-      <c r="E12">
+      <c r="F12">
         <v>108</v>
       </c>
-      <c r="F12">
+      <c r="G12">
         <v>124</v>
       </c>
-      <c r="G12">
+      <c r="H12">
         <v>123</v>
-      </c>
-      <c r="H12">
-        <v>111</v>
       </c>
       <c r="I12">
         <v>111</v>
       </c>
       <c r="J12">
+        <v>111</v>
+      </c>
+      <c r="K12">
         <v>110</v>
       </c>
-      <c r="K12">
+      <c r="L12">
         <v>83</v>
       </c>
-      <c r="L12">
+      <c r="M12">
         <v>201</v>
       </c>
-      <c r="M12">
+      <c r="N12">
         <v>175</v>
-      </c>
-      <c r="N12" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>25</v>
       </c>
-      <c r="B13">
-        <v>0</v>
+      <c r="B13" t="s">
+        <v>28</v>
       </c>
       <c r="C13">
         <v>0</v>
       </c>
       <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
         <v>4</v>
       </c>
-      <c r="E13">
+      <c r="F13">
         <v>13</v>
       </c>
-      <c r="F13">
+      <c r="G13">
         <v>9</v>
       </c>
-      <c r="G13">
+      <c r="H13">
         <v>48</v>
       </c>
-      <c r="H13">
+      <c r="I13">
         <v>40</v>
       </c>
-      <c r="I13">
+      <c r="J13">
         <v>3</v>
       </c>
-      <c r="J13">
+      <c r="K13">
         <v>40</v>
       </c>
-      <c r="K13">
+      <c r="L13">
         <v>31</v>
       </c>
-      <c r="L13">
+      <c r="M13">
         <v>29</v>
       </c>
-      <c r="M13">
+      <c r="N13">
         <v>17</v>
-      </c>
-      <c r="N13" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>26</v>
       </c>
-      <c r="B14">
+      <c r="B14" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14">
         <v>25</v>
       </c>
-      <c r="C14">
+      <c r="D14">
         <v>13</v>
       </c>
-      <c r="D14">
+      <c r="E14">
         <v>35</v>
       </c>
-      <c r="E14">
+      <c r="F14">
         <v>15</v>
       </c>
-      <c r="F14">
+      <c r="G14">
         <v>13</v>
       </c>
-      <c r="G14">
+      <c r="H14">
         <v>44</v>
       </c>
-      <c r="H14">
+      <c r="I14">
         <v>11</v>
       </c>
-      <c r="I14">
+      <c r="J14">
         <v>8</v>
       </c>
-      <c r="J14">
+      <c r="K14">
         <v>42</v>
       </c>
-      <c r="K14">
+      <c r="L14">
         <v>21</v>
       </c>
-      <c r="L14">
+      <c r="M14">
         <v>55</v>
       </c>
-      <c r="M14">
+      <c r="N14">
         <v>31</v>
-      </c>
-      <c r="N14" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>27</v>
       </c>
-      <c r="B15">
-        <v>0</v>
+      <c r="B15" t="s">
+        <v>28</v>
       </c>
       <c r="C15">
         <v>0</v>
@@ -1073,269 +1073,269 @@
         <v>0</v>
       </c>
       <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
         <v>2</v>
       </c>
-      <c r="H15">
+      <c r="I15">
         <v>1</v>
       </c>
-      <c r="I15">
-        <v>0</v>
-      </c>
       <c r="J15">
+        <v>0</v>
+      </c>
+      <c r="K15">
         <v>2</v>
       </c>
-      <c r="K15">
-        <v>0</v>
-      </c>
       <c r="L15">
         <v>0</v>
       </c>
       <c r="M15">
         <v>0</v>
       </c>
-      <c r="N15" t="s">
-        <v>28</v>
+      <c r="N15">
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>14</v>
       </c>
-      <c r="B16">
+      <c r="B16" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16">
         <v>1012</v>
       </c>
-      <c r="C16">
+      <c r="D16">
         <v>1821</v>
       </c>
-      <c r="D16">
+      <c r="E16">
         <v>2273</v>
       </c>
-      <c r="E16">
+      <c r="F16">
         <v>2277</v>
       </c>
-      <c r="F16">
+      <c r="G16">
         <v>1895</v>
       </c>
-      <c r="G16">
+      <c r="H16">
         <v>2121</v>
       </c>
-      <c r="H16">
+      <c r="I16">
         <v>2267</v>
       </c>
-      <c r="I16">
+      <c r="J16">
         <v>2387</v>
       </c>
-      <c r="J16">
+      <c r="K16">
         <v>2956</v>
       </c>
-      <c r="K16">
+      <c r="L16">
         <v>2914</v>
       </c>
-      <c r="L16">
+      <c r="M16">
         <v>3132</v>
       </c>
-      <c r="M16">
+      <c r="N16">
         <v>3488</v>
-      </c>
-      <c r="N16" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>15</v>
       </c>
-      <c r="B17">
+      <c r="B17" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17">
         <v>34</v>
       </c>
-      <c r="C17">
+      <c r="D17">
         <v>28</v>
       </c>
-      <c r="D17">
+      <c r="E17">
         <v>20</v>
       </c>
-      <c r="E17">
+      <c r="F17">
         <v>18</v>
       </c>
-      <c r="F17">
+      <c r="G17">
         <v>19</v>
       </c>
-      <c r="G17">
+      <c r="H17">
         <v>38</v>
       </c>
-      <c r="H17">
+      <c r="I17">
         <v>33</v>
       </c>
-      <c r="I17">
+      <c r="J17">
         <v>8</v>
       </c>
-      <c r="J17">
+      <c r="K17">
         <v>19</v>
       </c>
-      <c r="K17">
+      <c r="L17">
         <v>17</v>
       </c>
-      <c r="L17">
+      <c r="M17">
         <v>21</v>
       </c>
-      <c r="M17">
+      <c r="N17">
         <v>27</v>
-      </c>
-      <c r="N17" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>16</v>
       </c>
-      <c r="B18">
-        <v>0</v>
+      <c r="B18" t="s">
+        <v>29</v>
       </c>
       <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
         <v>142</v>
       </c>
-      <c r="D18">
+      <c r="E18">
         <v>247</v>
       </c>
-      <c r="E18">
+      <c r="F18">
         <v>253</v>
       </c>
-      <c r="F18">
+      <c r="G18">
         <v>197</v>
       </c>
-      <c r="G18">
+      <c r="H18">
         <v>341</v>
       </c>
-      <c r="H18">
+      <c r="I18">
         <v>203</v>
       </c>
-      <c r="I18">
+      <c r="J18">
         <v>251</v>
       </c>
-      <c r="J18">
+      <c r="K18">
         <v>792</v>
       </c>
-      <c r="K18">
+      <c r="L18">
         <v>625</v>
       </c>
-      <c r="L18">
+      <c r="M18">
         <v>837</v>
       </c>
-      <c r="M18">
+      <c r="N18">
         <v>671</v>
-      </c>
-      <c r="N18" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>17</v>
       </c>
-      <c r="B19">
+      <c r="B19" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19">
         <v>31</v>
       </c>
-      <c r="C19">
+      <c r="D19">
         <v>163</v>
       </c>
-      <c r="D19">
+      <c r="E19">
         <v>234</v>
       </c>
-      <c r="E19">
+      <c r="F19">
         <v>167</v>
       </c>
-      <c r="F19">
+      <c r="G19">
         <v>309</v>
       </c>
-      <c r="G19">
+      <c r="H19">
         <v>578</v>
       </c>
-      <c r="H19">
+      <c r="I19">
         <v>317</v>
       </c>
-      <c r="I19">
+      <c r="J19">
         <v>267</v>
       </c>
-      <c r="J19">
+      <c r="K19">
         <v>1159</v>
       </c>
-      <c r="K19">
+      <c r="L19">
         <v>1046</v>
       </c>
-      <c r="L19">
+      <c r="M19">
         <v>1757</v>
       </c>
-      <c r="M19">
+      <c r="N19">
         <v>1404</v>
-      </c>
-      <c r="N19" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>18</v>
       </c>
-      <c r="B20">
+      <c r="B20" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20">
         <v>131</v>
       </c>
-      <c r="C20">
+      <c r="D20">
         <v>137</v>
       </c>
-      <c r="D20">
+      <c r="E20">
         <v>132</v>
       </c>
-      <c r="E20">
+      <c r="F20">
         <v>116</v>
       </c>
-      <c r="F20">
+      <c r="G20">
         <v>219</v>
       </c>
-      <c r="G20">
+      <c r="H20">
         <v>340</v>
       </c>
-      <c r="H20">
+      <c r="I20">
         <v>250</v>
       </c>
-      <c r="I20">
+      <c r="J20">
         <v>181</v>
       </c>
-      <c r="J20">
+      <c r="K20">
         <v>600</v>
       </c>
-      <c r="K20">
+      <c r="L20">
         <v>537</v>
       </c>
-      <c r="L20">
+      <c r="M20">
         <v>817</v>
       </c>
-      <c r="M20">
+      <c r="N20">
         <v>558</v>
-      </c>
-      <c r="N20" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>19</v>
       </c>
-      <c r="B21">
-        <v>0</v>
+      <c r="B21" t="s">
+        <v>29</v>
       </c>
       <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
         <v>5</v>
       </c>
-      <c r="D21">
+      <c r="E21">
         <v>13</v>
       </c>
-      <c r="E21">
+      <c r="F21">
         <v>6</v>
       </c>
-      <c r="F21">
-        <v>0</v>
-      </c>
       <c r="G21">
         <v>0</v>
       </c>
@@ -1346,71 +1346,71 @@
         <v>0</v>
       </c>
       <c r="J21">
+        <v>0</v>
+      </c>
+      <c r="K21">
         <v>8</v>
       </c>
-      <c r="K21">
-        <v>0</v>
-      </c>
       <c r="L21">
         <v>0</v>
       </c>
       <c r="M21">
         <v>0</v>
       </c>
-      <c r="N21" t="s">
-        <v>29</v>
+      <c r="N21">
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>20</v>
       </c>
-      <c r="B22">
-        <v>0</v>
+      <c r="B22" t="s">
+        <v>29</v>
       </c>
       <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
         <v>24</v>
       </c>
-      <c r="D22">
+      <c r="E22">
         <v>196</v>
       </c>
-      <c r="E22">
+      <c r="F22">
         <v>143</v>
       </c>
-      <c r="F22">
+      <c r="G22">
         <v>127</v>
       </c>
-      <c r="G22">
+      <c r="H22">
         <v>209</v>
       </c>
-      <c r="H22">
+      <c r="I22">
         <v>159</v>
       </c>
-      <c r="I22">
+      <c r="J22">
         <v>145</v>
       </c>
-      <c r="J22">
+      <c r="K22">
         <v>519</v>
       </c>
-      <c r="K22">
+      <c r="L22">
         <v>421</v>
       </c>
-      <c r="L22">
+      <c r="M22">
         <v>493</v>
       </c>
-      <c r="M22">
+      <c r="N22">
         <v>391</v>
-      </c>
-      <c r="N22" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>21</v>
       </c>
-      <c r="B23">
-        <v>0</v>
+      <c r="B23" t="s">
+        <v>29</v>
       </c>
       <c r="C23">
         <v>0</v>
@@ -1434,247 +1434,247 @@
         <v>0</v>
       </c>
       <c r="J23">
+        <v>0</v>
+      </c>
+      <c r="K23">
         <v>3</v>
       </c>
-      <c r="K23">
+      <c r="L23">
         <v>14</v>
       </c>
-      <c r="L23">
+      <c r="M23">
         <v>18</v>
       </c>
-      <c r="M23">
+      <c r="N23">
         <v>6</v>
-      </c>
-      <c r="N23" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>22</v>
       </c>
-      <c r="B24">
+      <c r="B24" t="s">
+        <v>29</v>
+      </c>
+      <c r="C24">
         <v>460</v>
       </c>
-      <c r="C24">
+      <c r="D24">
         <v>455</v>
       </c>
-      <c r="D24">
+      <c r="E24">
         <v>524</v>
       </c>
-      <c r="E24">
+      <c r="F24">
         <v>457</v>
       </c>
-      <c r="F24">
+      <c r="G24">
         <v>692</v>
       </c>
-      <c r="G24">
+      <c r="H24">
         <v>882</v>
       </c>
-      <c r="H24">
+      <c r="I24">
         <v>631</v>
       </c>
-      <c r="I24">
+      <c r="J24">
         <v>574</v>
       </c>
-      <c r="J24">
+      <c r="K24">
         <v>1319</v>
       </c>
-      <c r="K24">
+      <c r="L24">
         <v>1101</v>
       </c>
-      <c r="L24">
+      <c r="M24">
         <v>1674</v>
       </c>
-      <c r="M24">
+      <c r="N24">
         <v>1433</v>
-      </c>
-      <c r="N24" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>23</v>
       </c>
-      <c r="B25">
+      <c r="B25" t="s">
+        <v>29</v>
+      </c>
+      <c r="C25">
         <v>9</v>
       </c>
-      <c r="C25">
+      <c r="D25">
         <v>14</v>
       </c>
-      <c r="D25">
+      <c r="E25">
         <v>56</v>
       </c>
-      <c r="E25">
+      <c r="F25">
         <v>32</v>
       </c>
-      <c r="F25">
+      <c r="G25">
         <v>10</v>
       </c>
-      <c r="G25">
+      <c r="H25">
         <v>69</v>
       </c>
-      <c r="H25">
+      <c r="I25">
         <v>33</v>
       </c>
-      <c r="I25">
+      <c r="J25">
         <v>12</v>
       </c>
-      <c r="J25">
+      <c r="K25">
         <v>82</v>
       </c>
-      <c r="K25">
+      <c r="L25">
         <v>29</v>
       </c>
-      <c r="L25">
+      <c r="M25">
         <v>15</v>
       </c>
-      <c r="M25">
+      <c r="N25">
         <v>9</v>
-      </c>
-      <c r="N25" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>24</v>
       </c>
-      <c r="B26">
+      <c r="B26" t="s">
+        <v>29</v>
+      </c>
+      <c r="C26">
         <v>152</v>
       </c>
-      <c r="C26">
+      <c r="D26">
         <v>131</v>
       </c>
-      <c r="D26">
+      <c r="E26">
         <v>143</v>
       </c>
-      <c r="E26">
+      <c r="F26">
         <v>106</v>
       </c>
-      <c r="F26">
+      <c r="G26">
         <v>119</v>
       </c>
-      <c r="G26">
+      <c r="H26">
         <v>112</v>
-      </c>
-      <c r="H26">
-        <v>106</v>
       </c>
       <c r="I26">
         <v>106</v>
       </c>
       <c r="J26">
+        <v>106</v>
+      </c>
+      <c r="K26">
         <v>110</v>
       </c>
-      <c r="K26">
+      <c r="L26">
         <v>84</v>
       </c>
-      <c r="L26">
+      <c r="M26">
         <v>161</v>
       </c>
-      <c r="M26">
+      <c r="N26">
         <v>121</v>
-      </c>
-      <c r="N26" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>25</v>
       </c>
-      <c r="B27">
-        <v>0</v>
+      <c r="B27" t="s">
+        <v>29</v>
       </c>
       <c r="C27">
         <v>0</v>
       </c>
       <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27">
         <v>1</v>
       </c>
-      <c r="E27">
+      <c r="F27">
         <v>10</v>
       </c>
-      <c r="F27">
+      <c r="G27">
         <v>7</v>
       </c>
-      <c r="G27">
+      <c r="H27">
         <v>37</v>
       </c>
-      <c r="H27">
+      <c r="I27">
         <v>32</v>
       </c>
-      <c r="I27">
+      <c r="J27">
         <v>3</v>
       </c>
-      <c r="J27">
+      <c r="K27">
         <v>31</v>
       </c>
-      <c r="K27">
+      <c r="L27">
         <v>22</v>
       </c>
-      <c r="L27">
+      <c r="M27">
         <v>23</v>
       </c>
-      <c r="M27">
+      <c r="N27">
         <v>13</v>
-      </c>
-      <c r="N27" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>26</v>
       </c>
-      <c r="B28">
+      <c r="B28" t="s">
+        <v>29</v>
+      </c>
+      <c r="C28">
         <v>19</v>
       </c>
-      <c r="C28">
+      <c r="D28">
         <v>10</v>
       </c>
-      <c r="D28">
+      <c r="E28">
         <v>24</v>
       </c>
-      <c r="E28">
+      <c r="F28">
         <v>12</v>
       </c>
-      <c r="F28">
+      <c r="G28">
         <v>11</v>
       </c>
-      <c r="G28">
+      <c r="H28">
         <v>35</v>
       </c>
-      <c r="H28">
+      <c r="I28">
         <v>6</v>
       </c>
-      <c r="I28">
+      <c r="J28">
         <v>7</v>
       </c>
-      <c r="J28">
+      <c r="K28">
         <v>26</v>
       </c>
-      <c r="K28">
+      <c r="L28">
         <v>15</v>
       </c>
-      <c r="L28">
+      <c r="M28">
         <v>36</v>
       </c>
-      <c r="M28">
+      <c r="N28">
         <v>25</v>
-      </c>
-      <c r="N28" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>27</v>
       </c>
-      <c r="B29">
-        <v>0</v>
+      <c r="B29" t="s">
+        <v>29</v>
       </c>
       <c r="C29">
         <v>0</v>
@@ -1692,266 +1692,266 @@
         <v>0</v>
       </c>
       <c r="H29">
+        <v>0</v>
+      </c>
+      <c r="I29">
         <v>1</v>
       </c>
-      <c r="I29">
-        <v>0</v>
-      </c>
       <c r="J29">
+        <v>0</v>
+      </c>
+      <c r="K29">
         <v>2</v>
       </c>
-      <c r="K29">
-        <v>0</v>
-      </c>
       <c r="L29">
         <v>0</v>
       </c>
       <c r="M29">
         <v>0</v>
       </c>
-      <c r="N29" t="s">
-        <v>29</v>
+      <c r="N29">
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>14</v>
       </c>
-      <c r="B30">
-        <v>0</v>
+      <c r="B30" t="s">
+        <v>30</v>
       </c>
       <c r="C30">
+        <v>0</v>
+      </c>
+      <c r="D30">
         <v>2288</v>
       </c>
-      <c r="D30">
+      <c r="E30">
         <v>3587</v>
       </c>
-      <c r="E30">
+      <c r="F30">
         <v>3638</v>
       </c>
-      <c r="F30">
+      <c r="G30">
         <v>3375</v>
       </c>
-      <c r="G30">
+      <c r="H30">
         <v>3676</v>
       </c>
-      <c r="H30">
+      <c r="I30">
         <v>3564</v>
       </c>
-      <c r="I30">
+      <c r="J30">
         <v>4013</v>
       </c>
-      <c r="J30">
+      <c r="K30">
         <v>4996</v>
       </c>
-      <c r="K30">
+      <c r="L30">
         <v>5029</v>
       </c>
-      <c r="L30">
+      <c r="M30">
         <v>5457</v>
       </c>
-      <c r="M30">
+      <c r="N30">
         <v>5843</v>
-      </c>
-      <c r="N30" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>15</v>
       </c>
-      <c r="B31">
-        <v>0</v>
+      <c r="B31" t="s">
+        <v>30</v>
       </c>
       <c r="C31">
+        <v>0</v>
+      </c>
+      <c r="D31">
         <v>41</v>
       </c>
-      <c r="D31">
+      <c r="E31">
         <v>40</v>
       </c>
-      <c r="E31">
+      <c r="F31">
         <v>53</v>
       </c>
-      <c r="F31">
+      <c r="G31">
         <v>59</v>
       </c>
-      <c r="G31">
+      <c r="H31">
         <v>70</v>
       </c>
-      <c r="H31">
+      <c r="I31">
         <v>86</v>
       </c>
-      <c r="I31">
+      <c r="J31">
         <v>50</v>
       </c>
-      <c r="J31">
+      <c r="K31">
         <v>61</v>
       </c>
-      <c r="K31">
+      <c r="L31">
         <v>53</v>
       </c>
-      <c r="L31">
+      <c r="M31">
         <v>50</v>
       </c>
-      <c r="M31">
+      <c r="N31">
         <v>73</v>
-      </c>
-      <c r="N31" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>16</v>
       </c>
-      <c r="B32">
-        <v>0</v>
+      <c r="B32" t="s">
+        <v>30</v>
       </c>
       <c r="C32">
+        <v>0</v>
+      </c>
+      <c r="D32">
         <v>300</v>
       </c>
-      <c r="D32">
+      <c r="E32">
         <v>1209</v>
       </c>
-      <c r="E32">
+      <c r="F32">
         <v>1568</v>
       </c>
-      <c r="F32">
+      <c r="G32">
         <v>2478</v>
       </c>
-      <c r="G32">
+      <c r="H32">
         <v>3187</v>
       </c>
-      <c r="H32">
+      <c r="I32">
         <v>3185</v>
       </c>
-      <c r="I32">
+      <c r="J32">
         <v>3200</v>
       </c>
-      <c r="J32">
+      <c r="K32">
         <v>6401</v>
       </c>
-      <c r="K32">
+      <c r="L32">
         <v>7208</v>
       </c>
-      <c r="L32">
+      <c r="M32">
         <v>9742</v>
       </c>
-      <c r="M32">
+      <c r="N32">
         <v>11202</v>
-      </c>
-      <c r="N32" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>17</v>
       </c>
-      <c r="B33">
-        <v>0</v>
+      <c r="B33" t="s">
+        <v>30</v>
       </c>
       <c r="C33">
+        <v>0</v>
+      </c>
+      <c r="D33">
         <v>1878</v>
       </c>
-      <c r="D33">
+      <c r="E33">
         <v>2611</v>
       </c>
-      <c r="E33">
+      <c r="F33">
         <v>2155</v>
       </c>
-      <c r="F33">
+      <c r="G33">
         <v>3040</v>
       </c>
-      <c r="G33">
+      <c r="H33">
         <v>4141</v>
       </c>
-      <c r="H33">
+      <c r="I33">
         <v>2820</v>
       </c>
-      <c r="I33">
+      <c r="J33">
         <v>2831</v>
       </c>
-      <c r="J33">
+      <c r="K33">
         <v>5772</v>
       </c>
-      <c r="K33">
+      <c r="L33">
         <v>6447</v>
       </c>
-      <c r="L33">
+      <c r="M33">
         <v>8419</v>
       </c>
-      <c r="M33">
+      <c r="N33">
         <v>9464</v>
-      </c>
-      <c r="N33" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>18</v>
       </c>
-      <c r="B34">
-        <v>0</v>
+      <c r="B34" t="s">
+        <v>30</v>
       </c>
       <c r="C34">
+        <v>0</v>
+      </c>
+      <c r="D34">
         <v>14843</v>
       </c>
-      <c r="D34">
+      <c r="E34">
         <v>21244</v>
       </c>
-      <c r="E34">
+      <c r="F34">
         <v>17905</v>
       </c>
-      <c r="F34">
+      <c r="G34">
         <v>25246</v>
       </c>
-      <c r="G34">
+      <c r="H34">
         <v>29945</v>
       </c>
-      <c r="H34">
+      <c r="I34">
         <v>20497</v>
       </c>
-      <c r="I34">
+      <c r="J34">
         <v>16712</v>
       </c>
-      <c r="J34">
+      <c r="K34">
         <v>33276</v>
       </c>
-      <c r="K34">
+      <c r="L34">
         <v>36074</v>
       </c>
-      <c r="L34">
+      <c r="M34">
         <v>42393</v>
       </c>
-      <c r="M34">
+      <c r="N34">
         <v>42102</v>
-      </c>
-      <c r="N34" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>19</v>
       </c>
-      <c r="B35">
-        <v>0</v>
+      <c r="B35" t="s">
+        <v>30</v>
       </c>
       <c r="C35">
+        <v>0</v>
+      </c>
+      <c r="D35">
         <v>9</v>
       </c>
-      <c r="D35">
+      <c r="E35">
         <v>27</v>
       </c>
-      <c r="E35">
+      <c r="F35">
         <v>2</v>
       </c>
-      <c r="F35">
-        <v>0</v>
-      </c>
       <c r="G35">
         <v>0</v>
       </c>
@@ -1962,71 +1962,71 @@
         <v>0</v>
       </c>
       <c r="J35">
+        <v>0</v>
+      </c>
+      <c r="K35">
         <v>4</v>
       </c>
-      <c r="K35">
-        <v>0</v>
-      </c>
       <c r="L35">
         <v>0</v>
       </c>
       <c r="M35">
         <v>0</v>
       </c>
-      <c r="N35" t="s">
-        <v>30</v>
+      <c r="N35">
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>20</v>
       </c>
-      <c r="B36">
-        <v>0</v>
+      <c r="B36" t="s">
+        <v>30</v>
       </c>
       <c r="C36">
+        <v>0</v>
+      </c>
+      <c r="D36">
         <v>95</v>
       </c>
-      <c r="D36">
+      <c r="E36">
         <v>727</v>
       </c>
-      <c r="E36">
+      <c r="F36">
         <v>1099</v>
       </c>
-      <c r="F36">
+      <c r="G36">
         <v>1445</v>
       </c>
-      <c r="G36">
+      <c r="H36">
         <v>2007</v>
       </c>
-      <c r="H36">
+      <c r="I36">
         <v>1980</v>
       </c>
-      <c r="I36">
+      <c r="J36">
         <v>1870</v>
       </c>
-      <c r="J36">
+      <c r="K36">
         <v>3642</v>
       </c>
-      <c r="K36">
+      <c r="L36">
         <v>4461</v>
       </c>
-      <c r="L36">
+      <c r="M36">
         <v>5806</v>
       </c>
-      <c r="M36">
+      <c r="N36">
         <v>6919</v>
-      </c>
-      <c r="N36" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>21</v>
       </c>
-      <c r="B37">
-        <v>0</v>
+      <c r="B37" t="s">
+        <v>30</v>
       </c>
       <c r="C37">
         <v>0</v>
@@ -2050,263 +2050,263 @@
         <v>0</v>
       </c>
       <c r="J37">
+        <v>0</v>
+      </c>
+      <c r="K37">
         <v>202</v>
       </c>
-      <c r="K37">
+      <c r="L37">
         <v>269</v>
       </c>
-      <c r="L37">
+      <c r="M37">
         <v>361</v>
       </c>
-      <c r="M37">
+      <c r="N37">
         <v>406</v>
-      </c>
-      <c r="N37" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>22</v>
       </c>
-      <c r="B38">
-        <v>0</v>
+      <c r="B38" t="s">
+        <v>30</v>
       </c>
       <c r="C38">
+        <v>0</v>
+      </c>
+      <c r="D38">
         <v>2773</v>
       </c>
-      <c r="D38">
+      <c r="E38">
         <v>4222</v>
       </c>
-      <c r="E38">
+      <c r="F38">
         <v>3524</v>
       </c>
-      <c r="F38">
+      <c r="G38">
         <v>5178</v>
       </c>
-      <c r="G38">
+      <c r="H38">
         <v>6227</v>
       </c>
-      <c r="H38">
+      <c r="I38">
         <v>5030</v>
       </c>
-      <c r="I38">
+      <c r="J38">
         <v>4161</v>
       </c>
-      <c r="J38">
+      <c r="K38">
         <v>8335</v>
       </c>
-      <c r="K38">
+      <c r="L38">
         <v>7431</v>
       </c>
-      <c r="L38">
+      <c r="M38">
         <v>9559</v>
       </c>
-      <c r="M38">
+      <c r="N38">
         <v>9058</v>
-      </c>
-      <c r="N38" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>23</v>
       </c>
-      <c r="B39">
-        <v>0</v>
+      <c r="B39" t="s">
+        <v>30</v>
       </c>
       <c r="C39">
+        <v>0</v>
+      </c>
+      <c r="D39">
         <v>11</v>
       </c>
-      <c r="D39">
+      <c r="E39">
         <v>46</v>
       </c>
-      <c r="E39">
+      <c r="F39">
         <v>24</v>
       </c>
-      <c r="F39">
+      <c r="G39">
         <v>1</v>
       </c>
-      <c r="G39">
+      <c r="H39">
         <v>43</v>
       </c>
-      <c r="H39">
+      <c r="I39">
         <v>19</v>
       </c>
-      <c r="I39">
+      <c r="J39">
         <v>10</v>
       </c>
-      <c r="J39">
+      <c r="K39">
         <v>50</v>
       </c>
-      <c r="K39">
+      <c r="L39">
         <v>18</v>
       </c>
-      <c r="L39">
-        <v>0</v>
-      </c>
       <c r="M39">
         <v>0</v>
       </c>
-      <c r="N39" t="s">
-        <v>30</v>
+      <c r="N39">
+        <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>24</v>
       </c>
-      <c r="B40">
+      <c r="B40" t="s">
+        <v>30</v>
+      </c>
+      <c r="C40">
         <v>24452</v>
       </c>
-      <c r="C40">
+      <c r="D40">
         <v>5994</v>
       </c>
-      <c r="D40">
+      <c r="E40">
         <v>438</v>
       </c>
-      <c r="E40">
+      <c r="F40">
         <v>299</v>
       </c>
-      <c r="F40">
+      <c r="G40">
         <v>478</v>
       </c>
-      <c r="G40">
+      <c r="H40">
         <v>527</v>
       </c>
-      <c r="H40">
+      <c r="I40">
         <v>344</v>
       </c>
-      <c r="I40">
+      <c r="J40">
         <v>259</v>
       </c>
-      <c r="J40">
+      <c r="K40">
         <v>339</v>
       </c>
-      <c r="K40">
+      <c r="L40">
         <v>275</v>
       </c>
-      <c r="L40">
+      <c r="M40">
         <v>986</v>
       </c>
-      <c r="M40">
+      <c r="N40">
         <v>540</v>
-      </c>
-      <c r="N40" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>25</v>
       </c>
-      <c r="B41">
-        <v>0</v>
+      <c r="B41" t="s">
+        <v>30</v>
       </c>
       <c r="C41">
         <v>0</v>
       </c>
       <c r="D41">
+        <v>0</v>
+      </c>
+      <c r="E41">
         <v>6</v>
       </c>
-      <c r="E41">
+      <c r="F41">
         <v>17</v>
       </c>
-      <c r="F41">
+      <c r="G41">
         <v>4</v>
       </c>
-      <c r="G41">
+      <c r="H41">
         <v>27</v>
       </c>
-      <c r="H41">
+      <c r="I41">
         <v>16</v>
       </c>
-      <c r="I41">
+      <c r="J41">
         <v>5</v>
       </c>
-      <c r="J41">
+      <c r="K41">
         <v>21</v>
       </c>
-      <c r="K41">
+      <c r="L41">
         <v>12</v>
       </c>
-      <c r="L41">
+      <c r="M41">
         <v>27</v>
       </c>
-      <c r="M41">
+      <c r="N41">
         <v>26</v>
-      </c>
-      <c r="N41" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>26</v>
       </c>
-      <c r="B42">
-        <v>0</v>
+      <c r="B42" t="s">
+        <v>30</v>
       </c>
       <c r="C42">
+        <v>0</v>
+      </c>
+      <c r="D42">
         <v>20</v>
       </c>
-      <c r="D42">
+      <c r="E42">
         <v>33</v>
       </c>
-      <c r="E42">
+      <c r="F42">
         <v>24</v>
       </c>
-      <c r="F42">
+      <c r="G42">
         <v>28</v>
       </c>
-      <c r="G42">
+      <c r="H42">
         <v>47</v>
       </c>
-      <c r="H42">
+      <c r="I42">
         <v>18</v>
       </c>
-      <c r="I42">
+      <c r="J42">
         <v>12</v>
       </c>
-      <c r="J42">
+      <c r="K42">
         <v>40</v>
       </c>
-      <c r="K42">
+      <c r="L42">
         <v>23</v>
-      </c>
-      <c r="L42">
-        <v>46</v>
       </c>
       <c r="M42">
         <v>46</v>
       </c>
-      <c r="N42" t="s">
-        <v>30</v>
+      <c r="N42">
+        <v>46</v>
       </c>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>27</v>
       </c>
-      <c r="B43">
-        <v>0</v>
+      <c r="B43" t="s">
+        <v>30</v>
       </c>
       <c r="C43">
         <v>0</v>
       </c>
       <c r="D43">
+        <v>0</v>
+      </c>
+      <c r="E43">
         <v>1</v>
       </c>
-      <c r="E43">
-        <v>0</v>
-      </c>
       <c r="F43">
+        <v>0</v>
+      </c>
+      <c r="G43">
         <v>1</v>
       </c>
-      <c r="G43">
-        <v>0</v>
-      </c>
       <c r="H43">
         <v>0</v>
       </c>
@@ -2314,19 +2314,19 @@
         <v>0</v>
       </c>
       <c r="J43">
+        <v>0</v>
+      </c>
+      <c r="K43">
         <v>2</v>
       </c>
-      <c r="K43">
+      <c r="L43">
         <v>1</v>
       </c>
-      <c r="L43">
-        <v>0</v>
-      </c>
       <c r="M43">
         <v>0</v>
       </c>
-      <c r="N43" t="s">
-        <v>30</v>
+      <c r="N43">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>